<commit_message>
wraped some long lines
</commit_message>
<xml_diff>
--- a/Excel/2021.08.07.xlsx
+++ b/Excel/2021.08.07.xlsx
@@ -11769,10 +11769,10 @@
         <v>94641</v>
       </c>
       <c r="D2" t="n">
-        <v>-12363</v>
+        <v>-12361</v>
       </c>
       <c r="E2" t="n">
-        <v>82278</v>
+        <v>82280</v>
       </c>
     </row>
     <row r="3">
@@ -11790,10 +11790,10 @@
         <v>77266</v>
       </c>
       <c r="D3" t="n">
-        <v>2981</v>
+        <v>2986</v>
       </c>
       <c r="E3" t="n">
-        <v>80247</v>
+        <v>80252</v>
       </c>
     </row>
     <row r="4">
@@ -11811,10 +11811,10 @@
         <v>63869</v>
       </c>
       <c r="D4" t="n">
-        <v>-3372</v>
+        <v>-3371</v>
       </c>
       <c r="E4" t="n">
-        <v>60497</v>
+        <v>60498</v>
       </c>
     </row>
     <row r="5">
@@ -11895,10 +11895,10 @@
         <v>33194</v>
       </c>
       <c r="D8" t="n">
-        <v>1430</v>
+        <v>1433</v>
       </c>
       <c r="E8" t="n">
-        <v>34624</v>
+        <v>34627</v>
       </c>
     </row>
     <row r="9">
@@ -11916,10 +11916,10 @@
         <v>30598</v>
       </c>
       <c r="D9" t="n">
-        <v>-3512</v>
+        <v>-3510</v>
       </c>
       <c r="E9" t="n">
-        <v>27086</v>
+        <v>27088</v>
       </c>
     </row>
     <row r="10">
@@ -11979,10 +11979,10 @@
         <v>26507</v>
       </c>
       <c r="D12" t="n">
-        <v>922</v>
+        <v>927</v>
       </c>
       <c r="E12" t="n">
-        <v>27429</v>
+        <v>27434</v>
       </c>
     </row>
     <row r="13">
@@ -12000,10 +12000,10 @@
         <v>26205</v>
       </c>
       <c r="D13" t="n">
-        <v>-7</v>
+        <v>-5</v>
       </c>
       <c r="E13" t="n">
-        <v>26198</v>
+        <v>26200</v>
       </c>
     </row>
     <row r="14">
@@ -12042,10 +12042,10 @@
         <v>22439</v>
       </c>
       <c r="D15" t="n">
-        <v>2922</v>
+        <v>2924</v>
       </c>
       <c r="E15" t="n">
-        <v>25361</v>
+        <v>25363</v>
       </c>
     </row>
     <row r="16">
@@ -12063,10 +12063,10 @@
         <v>21273</v>
       </c>
       <c r="D16" t="n">
-        <v>-37</v>
+        <v>-35</v>
       </c>
       <c r="E16" t="n">
-        <v>21236</v>
+        <v>21238</v>
       </c>
     </row>
     <row r="17">
@@ -12084,10 +12084,10 @@
         <v>21119</v>
       </c>
       <c r="D17" t="n">
-        <v>12209</v>
+        <v>12217</v>
       </c>
       <c r="E17" t="n">
-        <v>33328</v>
+        <v>33336</v>
       </c>
     </row>
     <row r="18">
@@ -12105,10 +12105,10 @@
         <v>20297</v>
       </c>
       <c r="D18" t="n">
-        <v>1289</v>
+        <v>1291</v>
       </c>
       <c r="E18" t="n">
-        <v>21586</v>
+        <v>21588</v>
       </c>
     </row>
     <row r="19">
@@ -12126,10 +12126,10 @@
         <v>20094</v>
       </c>
       <c r="D19" t="n">
-        <v>-506</v>
+        <v>-505</v>
       </c>
       <c r="E19" t="n">
-        <v>19588</v>
+        <v>19589</v>
       </c>
     </row>
     <row r="20">
@@ -12147,10 +12147,10 @@
         <v>18983</v>
       </c>
       <c r="D20" t="n">
-        <v>-785</v>
+        <v>-783</v>
       </c>
       <c r="E20" t="n">
-        <v>18198</v>
+        <v>18200</v>
       </c>
     </row>
     <row r="21" ht="28.8" customHeight="1">
@@ -12168,10 +12168,10 @@
         <v>18457</v>
       </c>
       <c r="D21" t="n">
-        <v>1293</v>
+        <v>1294</v>
       </c>
       <c r="E21" t="n">
-        <v>19750</v>
+        <v>19751</v>
       </c>
     </row>
     <row r="22">
@@ -12189,10 +12189,10 @@
         <v>17796</v>
       </c>
       <c r="D22" t="n">
-        <v>1115</v>
+        <v>1117</v>
       </c>
       <c r="E22" t="n">
-        <v>18911</v>
+        <v>18913</v>
       </c>
     </row>
     <row r="23">
@@ -12210,10 +12210,10 @@
         <v>17662</v>
       </c>
       <c r="D23" t="n">
-        <v>-348</v>
+        <v>-346</v>
       </c>
       <c r="E23" t="n">
-        <v>17314</v>
+        <v>17316</v>
       </c>
     </row>
     <row r="24">
@@ -12231,10 +12231,10 @@
         <v>17108</v>
       </c>
       <c r="D24" t="n">
-        <v>1898</v>
+        <v>1899</v>
       </c>
       <c r="E24" t="n">
-        <v>19006</v>
+        <v>19007</v>
       </c>
     </row>
     <row r="25">
@@ -12252,10 +12252,10 @@
         <v>16570</v>
       </c>
       <c r="D25" t="n">
-        <v>-377</v>
+        <v>-376</v>
       </c>
       <c r="E25" t="n">
-        <v>16193</v>
+        <v>16194</v>
       </c>
     </row>
     <row r="26">
@@ -12273,10 +12273,10 @@
         <v>16472</v>
       </c>
       <c r="D26" t="n">
-        <v>-1684</v>
+        <v>-1683</v>
       </c>
       <c r="E26" t="n">
-        <v>14788</v>
+        <v>14789</v>
       </c>
     </row>
     <row r="27">
@@ -12294,10 +12294,10 @@
         <v>15899</v>
       </c>
       <c r="D27" t="n">
-        <v>-687</v>
+        <v>-686</v>
       </c>
       <c r="E27" t="n">
-        <v>15212</v>
+        <v>15213</v>
       </c>
     </row>
     <row r="28">
@@ -12336,10 +12336,10 @@
         <v>14362</v>
       </c>
       <c r="D29" t="n">
-        <v>-1266</v>
+        <v>-1267</v>
       </c>
       <c r="E29" t="n">
-        <v>13096</v>
+        <v>13095</v>
       </c>
     </row>
     <row r="30">
@@ -12357,10 +12357,10 @@
         <v>13367</v>
       </c>
       <c r="D30" t="n">
-        <v>-362</v>
+        <v>-361</v>
       </c>
       <c r="E30" t="n">
-        <v>13005</v>
+        <v>13006</v>
       </c>
     </row>
     <row r="31">
@@ -12378,10 +12378,10 @@
         <v>13322</v>
       </c>
       <c r="D31" t="n">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="E31" t="n">
-        <v>13755</v>
+        <v>13757</v>
       </c>
     </row>
     <row r="32">
@@ -12462,10 +12462,10 @@
         <v>12783</v>
       </c>
       <c r="D35" t="n">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E35" t="n">
-        <v>13039</v>
+        <v>13040</v>
       </c>
     </row>
     <row r="36">
@@ -12483,10 +12483,10 @@
         <v>12530</v>
       </c>
       <c r="D36" t="n">
-        <v>-1201</v>
+        <v>-1202</v>
       </c>
       <c r="E36" t="n">
-        <v>11329</v>
+        <v>11328</v>
       </c>
     </row>
     <row r="37">
@@ -12546,10 +12546,10 @@
         <v>11175</v>
       </c>
       <c r="D39" t="n">
-        <v>-729</v>
+        <v>-728</v>
       </c>
       <c r="E39" t="n">
-        <v>10446</v>
+        <v>10447</v>
       </c>
     </row>
     <row r="40">
@@ -12567,10 +12567,10 @@
         <v>11172</v>
       </c>
       <c r="D40" t="n">
-        <v>-105</v>
+        <v>-104</v>
       </c>
       <c r="E40" t="n">
-        <v>11067</v>
+        <v>11068</v>
       </c>
     </row>
     <row r="41">
@@ -12609,10 +12609,10 @@
         <v>10695</v>
       </c>
       <c r="D42" t="n">
-        <v>1033</v>
+        <v>1035</v>
       </c>
       <c r="E42" t="n">
-        <v>11728</v>
+        <v>11730</v>
       </c>
     </row>
     <row r="43">
@@ -12651,10 +12651,10 @@
         <v>10622</v>
       </c>
       <c r="D44" t="n">
-        <v>-54</v>
+        <v>-52</v>
       </c>
       <c r="E44" t="n">
-        <v>10568</v>
+        <v>10570</v>
       </c>
     </row>
     <row r="45">
@@ -12672,10 +12672,10 @@
         <v>10462</v>
       </c>
       <c r="D45" t="n">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E45" t="n">
-        <v>10641</v>
+        <v>10645</v>
       </c>
     </row>
     <row r="46">
@@ -12693,10 +12693,10 @@
         <v>10446</v>
       </c>
       <c r="D46" t="n">
-        <v>-164</v>
+        <v>-161</v>
       </c>
       <c r="E46" t="n">
-        <v>10282</v>
+        <v>10285</v>
       </c>
     </row>
     <row r="47">
@@ -12735,10 +12735,10 @@
         <v>9811</v>
       </c>
       <c r="D48" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E48" t="n">
-        <v>9876</v>
+        <v>9877</v>
       </c>
     </row>
     <row r="49">
@@ -12799,7 +12799,7 @@
       </c>
       <c r="C52" s="11" t="n"/>
       <c r="E52" t="n">
-        <v>13124</v>
+        <v>13127</v>
       </c>
     </row>
     <row r="53">
@@ -12831,7 +12831,7 @@
       </c>
       <c r="C54" s="11" t="n"/>
       <c r="E54" t="n">
-        <v>9360</v>
+        <v>9361</v>
       </c>
     </row>
     <row r="55">

</xml_diff>

<commit_message>
wraped all too long lines
</commit_message>
<xml_diff>
--- a/Excel/2021.08.07.xlsx
+++ b/Excel/2021.08.07.xlsx
@@ -24026,10 +24026,10 @@
         <v>1456415</v>
       </c>
       <c r="R32" t="n">
-        <v>134096</v>
+        <v>134401</v>
       </c>
       <c r="S32" t="n">
-        <v>1590511</v>
+        <v>1590816</v>
       </c>
     </row>
     <row r="33">
@@ -33629,10 +33629,10 @@
         <v>194251</v>
       </c>
       <c r="D2" t="n">
-        <v>-12075</v>
+        <v>-12067</v>
       </c>
       <c r="E2" t="n">
-        <v>182176</v>
+        <v>182184</v>
       </c>
     </row>
     <row r="3">
@@ -33650,10 +33650,10 @@
         <v>161956</v>
       </c>
       <c r="D3" t="n">
-        <v>-5121</v>
+        <v>-5111</v>
       </c>
       <c r="E3" t="n">
-        <v>156835</v>
+        <v>156845</v>
       </c>
     </row>
     <row r="4">
@@ -33671,10 +33671,10 @@
         <v>156450</v>
       </c>
       <c r="D4" t="n">
-        <v>-1756</v>
+        <v>-1753</v>
       </c>
       <c r="E4" t="n">
-        <v>154694</v>
+        <v>154697</v>
       </c>
     </row>
     <row r="5">
@@ -33692,10 +33692,10 @@
         <v>155992</v>
       </c>
       <c r="D5" t="n">
-        <v>-19030</v>
+        <v>-19028</v>
       </c>
       <c r="E5" t="n">
-        <v>136962</v>
+        <v>136964</v>
       </c>
     </row>
     <row r="6">
@@ -33713,10 +33713,10 @@
         <v>145866</v>
       </c>
       <c r="D6" t="n">
-        <v>-14216</v>
+        <v>-14210</v>
       </c>
       <c r="E6" t="n">
-        <v>131650</v>
+        <v>131656</v>
       </c>
     </row>
     <row r="7">
@@ -33734,10 +33734,10 @@
         <v>139632</v>
       </c>
       <c r="D7" t="n">
-        <v>-10721</v>
+        <v>-10712</v>
       </c>
       <c r="E7" t="n">
-        <v>128911</v>
+        <v>128920</v>
       </c>
     </row>
     <row r="8">
@@ -33776,10 +33776,10 @@
         <v>93126</v>
       </c>
       <c r="D9" t="n">
-        <v>-12180</v>
+        <v>-12175</v>
       </c>
       <c r="E9" t="n">
-        <v>80946</v>
+        <v>80951</v>
       </c>
     </row>
     <row r="10">
@@ -33797,10 +33797,10 @@
         <v>78250</v>
       </c>
       <c r="D10" t="n">
-        <v>-16339</v>
+        <v>-16337</v>
       </c>
       <c r="E10" t="n">
-        <v>61911</v>
+        <v>61913</v>
       </c>
     </row>
     <row r="11">
@@ -33818,10 +33818,10 @@
         <v>76955</v>
       </c>
       <c r="D11" t="n">
-        <v>-905</v>
+        <v>-902</v>
       </c>
       <c r="E11" t="n">
-        <v>76050</v>
+        <v>76053</v>
       </c>
     </row>
     <row r="12">
@@ -33839,10 +33839,10 @@
         <v>75805</v>
       </c>
       <c r="D12" t="n">
-        <v>-3150</v>
+        <v>-3147</v>
       </c>
       <c r="E12" t="n">
-        <v>72655</v>
+        <v>72658</v>
       </c>
     </row>
     <row r="13">
@@ -33860,10 +33860,10 @@
         <v>74500</v>
       </c>
       <c r="D13" t="n">
-        <v>-2792</v>
+        <v>-2788</v>
       </c>
       <c r="E13" t="n">
-        <v>71708</v>
+        <v>71712</v>
       </c>
     </row>
     <row r="14">
@@ -33881,10 +33881,10 @@
         <v>72046</v>
       </c>
       <c r="D14" t="n">
-        <v>-12979</v>
+        <v>-12975</v>
       </c>
       <c r="E14" t="n">
-        <v>59067</v>
+        <v>59071</v>
       </c>
     </row>
     <row r="15">
@@ -33902,10 +33902,10 @@
         <v>70294</v>
       </c>
       <c r="D15" t="n">
-        <v>-3181</v>
+        <v>-3180</v>
       </c>
       <c r="E15" t="n">
-        <v>67113</v>
+        <v>67114</v>
       </c>
     </row>
     <row r="16">
@@ -33944,10 +33944,10 @@
         <v>68315</v>
       </c>
       <c r="D17" t="n">
-        <v>-4232</v>
+        <v>-4226</v>
       </c>
       <c r="E17" t="n">
-        <v>64083</v>
+        <v>64089</v>
       </c>
     </row>
     <row r="18">
@@ -33965,10 +33965,10 @@
         <v>67934</v>
       </c>
       <c r="D18" t="n">
-        <v>-5880</v>
+        <v>-5879</v>
       </c>
       <c r="E18" t="n">
-        <v>62054</v>
+        <v>62055</v>
       </c>
     </row>
     <row r="19">
@@ -33986,10 +33986,10 @@
         <v>67763</v>
       </c>
       <c r="D19" t="n">
-        <v>-2986</v>
+        <v>-2988</v>
       </c>
       <c r="E19" t="n">
-        <v>64777</v>
+        <v>64775</v>
       </c>
     </row>
     <row r="20">
@@ -34028,10 +34028,10 @@
         <v>63425</v>
       </c>
       <c r="D21" t="n">
-        <v>-17278</v>
+        <v>-17272</v>
       </c>
       <c r="E21" t="n">
-        <v>46147</v>
+        <v>46153</v>
       </c>
     </row>
     <row r="22">
@@ -34049,10 +34049,10 @@
         <v>60083</v>
       </c>
       <c r="D22" t="n">
-        <v>-2167</v>
+        <v>-2165</v>
       </c>
       <c r="E22" t="n">
-        <v>57916</v>
+        <v>57918</v>
       </c>
     </row>
     <row r="23">
@@ -34070,10 +34070,10 @@
         <v>57384</v>
       </c>
       <c r="D23" t="n">
-        <v>-7654</v>
+        <v>-7653</v>
       </c>
       <c r="E23" t="n">
-        <v>49730</v>
+        <v>49731</v>
       </c>
     </row>
     <row r="24">
@@ -34091,10 +34091,10 @@
         <v>57239</v>
       </c>
       <c r="D24" t="n">
-        <v>-5345</v>
+        <v>-5343</v>
       </c>
       <c r="E24" t="n">
-        <v>51894</v>
+        <v>51896</v>
       </c>
     </row>
     <row r="25">
@@ -34112,10 +34112,10 @@
         <v>57190</v>
       </c>
       <c r="D25" t="n">
-        <v>-2183</v>
+        <v>-2186</v>
       </c>
       <c r="E25" t="n">
-        <v>55007</v>
+        <v>55004</v>
       </c>
     </row>
     <row r="26">
@@ -34133,10 +34133,10 @@
         <v>54383</v>
       </c>
       <c r="D26" t="n">
-        <v>-5596</v>
+        <v>-5597</v>
       </c>
       <c r="E26" t="n">
-        <v>48787</v>
+        <v>48786</v>
       </c>
     </row>
     <row r="27">
@@ -34175,10 +34175,10 @@
         <v>50496</v>
       </c>
       <c r="D28" t="n">
-        <v>-1309</v>
+        <v>-1308</v>
       </c>
       <c r="E28" t="n">
-        <v>49187</v>
+        <v>49188</v>
       </c>
     </row>
     <row r="29">
@@ -34217,10 +34217,10 @@
         <v>48976</v>
       </c>
       <c r="D30" t="n">
-        <v>-6877</v>
+        <v>-6879</v>
       </c>
       <c r="E30" t="n">
-        <v>42099</v>
+        <v>42097</v>
       </c>
     </row>
     <row r="31">
@@ -34238,10 +34238,10 @@
         <v>48036</v>
       </c>
       <c r="D31" t="n">
-        <v>-6858</v>
+        <v>-6856</v>
       </c>
       <c r="E31" t="n">
-        <v>41178</v>
+        <v>41180</v>
       </c>
     </row>
     <row r="32">
@@ -34259,10 +34259,10 @@
         <v>47915</v>
       </c>
       <c r="D32" t="n">
-        <v>-5810</v>
+        <v>-5806</v>
       </c>
       <c r="E32" t="n">
-        <v>42105</v>
+        <v>42109</v>
       </c>
     </row>
     <row r="33">
@@ -34301,10 +34301,10 @@
         <v>47193</v>
       </c>
       <c r="D34" t="n">
-        <v>-3478</v>
+        <v>-3477</v>
       </c>
       <c r="E34" t="n">
-        <v>43715</v>
+        <v>43716</v>
       </c>
     </row>
     <row r="35">
@@ -34322,10 +34322,10 @@
         <v>45617</v>
       </c>
       <c r="D35" t="n">
-        <v>4095</v>
+        <v>4103</v>
       </c>
       <c r="E35" t="n">
-        <v>49712</v>
+        <v>49720</v>
       </c>
     </row>
     <row r="36">
@@ -34343,10 +34343,10 @@
         <v>43189</v>
       </c>
       <c r="D36" t="n">
-        <v>-523</v>
+        <v>-520</v>
       </c>
       <c r="E36" t="n">
-        <v>42666</v>
+        <v>42669</v>
       </c>
     </row>
     <row r="37">
@@ -34364,10 +34364,10 @@
         <v>40092</v>
       </c>
       <c r="D37" t="n">
-        <v>-1268</v>
+        <v>-1266</v>
       </c>
       <c r="E37" t="n">
-        <v>38824</v>
+        <v>38826</v>
       </c>
     </row>
     <row r="38">
@@ -34385,10 +34385,10 @@
         <v>39409</v>
       </c>
       <c r="D38" t="n">
-        <v>1416</v>
+        <v>1420</v>
       </c>
       <c r="E38" t="n">
-        <v>40825</v>
+        <v>40829</v>
       </c>
     </row>
     <row r="39" ht="28.8" customHeight="1">
@@ -34448,10 +34448,10 @@
         <v>36165</v>
       </c>
       <c r="D41" t="n">
-        <v>-3531</v>
+        <v>-3530</v>
       </c>
       <c r="E41" t="n">
-        <v>32634</v>
+        <v>32635</v>
       </c>
     </row>
     <row r="42">
@@ -34469,10 +34469,10 @@
         <v>34465</v>
       </c>
       <c r="D42" t="n">
-        <v>-4953</v>
+        <v>-4954</v>
       </c>
       <c r="E42" t="n">
-        <v>29512</v>
+        <v>29511</v>
       </c>
     </row>
     <row r="43" ht="28.8" customHeight="1">
@@ -34490,10 +34490,10 @@
         <v>34081</v>
       </c>
       <c r="D43" t="n">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="E43" t="n">
-        <v>34749</v>
+        <v>34750</v>
       </c>
     </row>
     <row r="44">
@@ -34511,10 +34511,10 @@
         <v>33808</v>
       </c>
       <c r="D44" t="n">
-        <v>-4729</v>
+        <v>-4728</v>
       </c>
       <c r="E44" t="n">
-        <v>29079</v>
+        <v>29080</v>
       </c>
     </row>
     <row r="45">
@@ -34616,10 +34616,10 @@
         <v>31457</v>
       </c>
       <c r="D49" t="n">
-        <v>-1545</v>
+        <v>-1543</v>
       </c>
       <c r="E49" t="n">
-        <v>29912</v>
+        <v>29914</v>
       </c>
     </row>
     <row r="50">
@@ -34658,10 +34658,10 @@
         <v>30864</v>
       </c>
       <c r="D51" t="n">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E51" t="n">
-        <v>31185</v>
+        <v>31186</v>
       </c>
     </row>
     <row r="52">
@@ -38974,10 +38974,10 @@
         <v>8.710000000000001</v>
       </c>
       <c r="P41" t="n">
-        <v>0</v>
+        <v>-0.01000000000000156</v>
       </c>
       <c r="Q41" t="n">
-        <v>8.710000000000001</v>
+        <v>8.699999999999999</v>
       </c>
     </row>
     <row r="42">
@@ -48265,10 +48265,10 @@
         <v>450539</v>
       </c>
       <c r="L2" t="n">
-        <v>48105</v>
+        <v>48125</v>
       </c>
       <c r="M2" t="n">
-        <v>498644</v>
+        <v>498664</v>
       </c>
     </row>
     <row r="3">
@@ -48310,10 +48310,10 @@
         <v>380452</v>
       </c>
       <c r="L3" t="n">
-        <v>29886</v>
+        <v>29901</v>
       </c>
       <c r="M3" t="n">
-        <v>410338</v>
+        <v>410353</v>
       </c>
     </row>
     <row r="4">
@@ -48355,10 +48355,10 @@
         <v>337956</v>
       </c>
       <c r="L4" t="n">
-        <v>12577</v>
+        <v>12588</v>
       </c>
       <c r="M4" t="n">
-        <v>350533</v>
+        <v>350544</v>
       </c>
     </row>
     <row r="5">
@@ -48400,10 +48400,10 @@
         <v>384868</v>
       </c>
       <c r="L5" t="n">
-        <v>42790</v>
+        <v>42809</v>
       </c>
       <c r="M5" t="n">
-        <v>427658</v>
+        <v>427677</v>
       </c>
     </row>
     <row r="6">
@@ -48445,10 +48445,10 @@
         <v>341927</v>
       </c>
       <c r="L6" t="n">
-        <v>28524</v>
+        <v>28542</v>
       </c>
       <c r="M6" t="n">
-        <v>370451</v>
+        <v>370469</v>
       </c>
     </row>
     <row r="7">
@@ -48490,10 +48490,10 @@
         <v>304166</v>
       </c>
       <c r="L7" t="n">
-        <v>25293</v>
+        <v>25311</v>
       </c>
       <c r="M7" t="n">
-        <v>329459</v>
+        <v>329477</v>
       </c>
     </row>
     <row r="8">
@@ -48535,10 +48535,10 @@
         <v>297432</v>
       </c>
       <c r="L8" t="n">
-        <v>18348</v>
+        <v>18364</v>
       </c>
       <c r="M8" t="n">
-        <v>315780</v>
+        <v>315796</v>
       </c>
     </row>
     <row r="9">
@@ -48580,10 +48580,10 @@
         <v>277021</v>
       </c>
       <c r="L9" t="n">
-        <v>11831</v>
+        <v>11842</v>
       </c>
       <c r="M9" t="n">
-        <v>288852</v>
+        <v>288863</v>
       </c>
     </row>
     <row r="10">
@@ -48625,10 +48625,10 @@
         <v>301800</v>
       </c>
       <c r="L10" t="n">
-        <v>30683</v>
+        <v>30700</v>
       </c>
       <c r="M10" t="n">
-        <v>332483</v>
+        <v>332500</v>
       </c>
     </row>
     <row r="11">
@@ -48670,10 +48670,10 @@
         <v>236707</v>
       </c>
       <c r="L11" t="n">
-        <v>5720</v>
+        <v>5723</v>
       </c>
       <c r="M11" t="n">
-        <v>242427</v>
+        <v>242430</v>
       </c>
     </row>
     <row r="12">
@@ -48715,10 +48715,10 @@
         <v>225793</v>
       </c>
       <c r="L12" t="n">
-        <v>11089</v>
+        <v>11096</v>
       </c>
       <c r="M12" t="n">
-        <v>236882</v>
+        <v>236889</v>
       </c>
     </row>
     <row r="13">
@@ -48760,10 +48760,10 @@
         <v>248346</v>
       </c>
       <c r="L13" t="n">
-        <v>27809</v>
+        <v>27816</v>
       </c>
       <c r="M13" t="n">
-        <v>276155</v>
+        <v>276162</v>
       </c>
     </row>
     <row r="14">
@@ -48805,10 +48805,10 @@
         <v>208489</v>
       </c>
       <c r="L14" t="n">
-        <v>10785</v>
+        <v>10792</v>
       </c>
       <c r="M14" t="n">
-        <v>219274</v>
+        <v>219281</v>
       </c>
     </row>
     <row r="15">
@@ -48850,10 +48850,10 @@
         <v>240290</v>
       </c>
       <c r="L15" t="n">
-        <v>19563</v>
+        <v>19573</v>
       </c>
       <c r="M15" t="n">
-        <v>259853</v>
+        <v>259863</v>
       </c>
     </row>
     <row r="16">
@@ -48895,10 +48895,10 @@
         <v>195713</v>
       </c>
       <c r="L16" t="n">
-        <v>14730</v>
+        <v>14742</v>
       </c>
       <c r="M16" t="n">
-        <v>210443</v>
+        <v>210455</v>
       </c>
     </row>
     <row r="17">
@@ -48940,10 +48940,10 @@
         <v>182779</v>
       </c>
       <c r="L17" t="n">
-        <v>13166</v>
+        <v>13172</v>
       </c>
       <c r="M17" t="n">
-        <v>195945</v>
+        <v>195951</v>
       </c>
     </row>
     <row r="18">
@@ -48985,10 +48985,10 @@
         <v>213218</v>
       </c>
       <c r="L18" t="n">
-        <v>21242</v>
+        <v>21248</v>
       </c>
       <c r="M18" t="n">
-        <v>234460</v>
+        <v>234466</v>
       </c>
     </row>
     <row r="19">
@@ -49030,10 +49030,10 @@
         <v>165782</v>
       </c>
       <c r="L19" t="n">
-        <v>6352</v>
+        <v>6354</v>
       </c>
       <c r="M19" t="n">
-        <v>172134</v>
+        <v>172136</v>
       </c>
     </row>
     <row r="20">
@@ -49075,10 +49075,10 @@
         <v>156042</v>
       </c>
       <c r="L20" t="n">
-        <v>4376</v>
+        <v>4384</v>
       </c>
       <c r="M20" t="n">
-        <v>160418</v>
+        <v>160426</v>
       </c>
     </row>
     <row r="21">
@@ -49120,10 +49120,10 @@
         <v>162215</v>
       </c>
       <c r="L21" t="n">
-        <v>8774</v>
+        <v>8776</v>
       </c>
       <c r="M21" t="n">
-        <v>170989</v>
+        <v>170991</v>
       </c>
     </row>
     <row r="22">
@@ -49165,10 +49165,10 @@
         <v>159857</v>
       </c>
       <c r="L22" t="n">
-        <v>7783</v>
+        <v>7789</v>
       </c>
       <c r="M22" t="n">
-        <v>167640</v>
+        <v>167646</v>
       </c>
     </row>
     <row r="23">
@@ -49210,10 +49210,10 @@
         <v>187278</v>
       </c>
       <c r="L23" t="n">
-        <v>23931</v>
+        <v>23941</v>
       </c>
       <c r="M23" t="n">
-        <v>211209</v>
+        <v>211219</v>
       </c>
     </row>
     <row r="24">
@@ -49255,10 +49255,10 @@
         <v>201921</v>
       </c>
       <c r="L24" t="n">
-        <v>43394</v>
+        <v>43411</v>
       </c>
       <c r="M24" t="n">
-        <v>245315</v>
+        <v>245332</v>
       </c>
     </row>
     <row r="25">
@@ -49300,10 +49300,10 @@
         <v>148222</v>
       </c>
       <c r="L25" t="n">
-        <v>6952</v>
+        <v>6956</v>
       </c>
       <c r="M25" t="n">
-        <v>155174</v>
+        <v>155178</v>
       </c>
     </row>
     <row r="26">
@@ -49345,10 +49345,10 @@
         <v>141447</v>
       </c>
       <c r="L26" t="n">
-        <v>6485</v>
+        <v>6487</v>
       </c>
       <c r="M26" t="n">
-        <v>147932</v>
+        <v>147934</v>
       </c>
     </row>
     <row r="27">
@@ -49390,10 +49390,10 @@
         <v>139201</v>
       </c>
       <c r="L27" t="n">
-        <v>6014</v>
+        <v>6018</v>
       </c>
       <c r="M27" t="n">
-        <v>145215</v>
+        <v>145219</v>
       </c>
     </row>
     <row r="28">
@@ -49435,10 +49435,10 @@
         <v>142048</v>
       </c>
       <c r="L28" t="n">
-        <v>6355</v>
+        <v>6358</v>
       </c>
       <c r="M28" t="n">
-        <v>148403</v>
+        <v>148406</v>
       </c>
     </row>
     <row r="29">
@@ -49480,10 +49480,10 @@
         <v>161498</v>
       </c>
       <c r="L29" t="n">
-        <v>19616</v>
+        <v>19625</v>
       </c>
       <c r="M29" t="n">
-        <v>181114</v>
+        <v>181123</v>
       </c>
     </row>
     <row r="30">
@@ -49525,10 +49525,10 @@
         <v>137303</v>
       </c>
       <c r="L30" t="n">
-        <v>8226</v>
+        <v>8231</v>
       </c>
       <c r="M30" t="n">
-        <v>145529</v>
+        <v>145534</v>
       </c>
     </row>
     <row r="31">
@@ -49570,10 +49570,10 @@
         <v>130378</v>
       </c>
       <c r="L31" t="n">
-        <v>5842</v>
+        <v>5844</v>
       </c>
       <c r="M31" t="n">
-        <v>136220</v>
+        <v>136222</v>
       </c>
     </row>
     <row r="32">
@@ -49615,10 +49615,10 @@
         <v>133068</v>
       </c>
       <c r="L32" t="n">
-        <v>7808</v>
+        <v>7816</v>
       </c>
       <c r="M32" t="n">
-        <v>140876</v>
+        <v>140884</v>
       </c>
     </row>
     <row r="33">
@@ -49660,10 +49660,10 @@
         <v>127496</v>
       </c>
       <c r="L33" t="n">
-        <v>4978</v>
+        <v>4981</v>
       </c>
       <c r="M33" t="n">
-        <v>132474</v>
+        <v>132477</v>
       </c>
     </row>
     <row r="34">
@@ -49705,10 +49705,10 @@
         <v>127209</v>
       </c>
       <c r="L34" t="n">
-        <v>4947</v>
+        <v>4949</v>
       </c>
       <c r="M34" t="n">
-        <v>132156</v>
+        <v>132158</v>
       </c>
     </row>
     <row r="35">
@@ -49795,10 +49795,10 @@
         <v>127352</v>
       </c>
       <c r="L36" t="n">
-        <v>6721</v>
+        <v>6725</v>
       </c>
       <c r="M36" t="n">
-        <v>134073</v>
+        <v>134077</v>
       </c>
     </row>
     <row r="37">
@@ -49840,10 +49840,10 @@
         <v>133807</v>
       </c>
       <c r="L37" t="n">
-        <v>9836</v>
+        <v>9843</v>
       </c>
       <c r="M37" t="n">
-        <v>143643</v>
+        <v>143650</v>
       </c>
     </row>
     <row r="38" ht="28.8" customHeight="1">
@@ -49885,10 +49885,10 @@
         <v>154775</v>
       </c>
       <c r="L38" t="n">
-        <v>19826</v>
+        <v>19835</v>
       </c>
       <c r="M38" t="n">
-        <v>174601</v>
+        <v>174610</v>
       </c>
     </row>
     <row r="39">
@@ -49930,10 +49930,10 @@
         <v>203853</v>
       </c>
       <c r="L39" t="n">
-        <v>50844</v>
+        <v>50870</v>
       </c>
       <c r="M39" t="n">
-        <v>254697</v>
+        <v>254723</v>
       </c>
     </row>
     <row r="40">
@@ -49975,10 +49975,10 @@
         <v>134344</v>
       </c>
       <c r="L40" t="n">
-        <v>12056</v>
+        <v>12061</v>
       </c>
       <c r="M40" t="n">
-        <v>146400</v>
+        <v>146405</v>
       </c>
     </row>
     <row r="41">
@@ -50020,10 +50020,10 @@
         <v>134582</v>
       </c>
       <c r="L41" t="n">
-        <v>14097</v>
+        <v>14104</v>
       </c>
       <c r="M41" t="n">
-        <v>148679</v>
+        <v>148686</v>
       </c>
     </row>
     <row r="42">
@@ -50065,10 +50065,10 @@
         <v>122218</v>
       </c>
       <c r="L42" t="n">
-        <v>7147</v>
+        <v>7153</v>
       </c>
       <c r="M42" t="n">
-        <v>129365</v>
+        <v>129371</v>
       </c>
     </row>
     <row r="43" ht="28.8" customHeight="1">
@@ -50110,10 +50110,10 @@
         <v>144062</v>
       </c>
       <c r="L43" t="n">
-        <v>16575</v>
+        <v>16582</v>
       </c>
       <c r="M43" t="n">
-        <v>160637</v>
+        <v>160644</v>
       </c>
     </row>
     <row r="44">
@@ -50190,10 +50190,10 @@
         <v>130904</v>
       </c>
       <c r="L45" t="n">
-        <v>16106</v>
+        <v>16113</v>
       </c>
       <c r="M45" t="n">
-        <v>147010</v>
+        <v>147017</v>
       </c>
     </row>
     <row r="46">
@@ -50270,10 +50270,10 @@
         <v>139067</v>
       </c>
       <c r="L47" t="n">
-        <v>22525</v>
+        <v>22533</v>
       </c>
       <c r="M47" t="n">
-        <v>161592</v>
+        <v>161600</v>
       </c>
     </row>
     <row r="48">
@@ -50424,10 +50424,10 @@
         <v>134397</v>
       </c>
       <c r="L51" t="n">
-        <v>15228</v>
+        <v>15238</v>
       </c>
       <c r="M51" t="n">
-        <v>149625</v>
+        <v>149635</v>
       </c>
     </row>
     <row r="52">
@@ -50453,10 +50453,10 @@
         <v>167772</v>
       </c>
       <c r="L52" t="n">
-        <v>90882</v>
+        <v>90933</v>
       </c>
       <c r="M52" t="n">
-        <v>258654</v>
+        <v>258705</v>
       </c>
     </row>
     <row r="53" ht="28.8" customHeight="1">
@@ -50482,10 +50482,10 @@
         <v>131436</v>
       </c>
       <c r="L53" t="n">
-        <v>13785</v>
+        <v>13790</v>
       </c>
       <c r="M53" t="n">
-        <v>145221</v>
+        <v>145226</v>
       </c>
     </row>
     <row r="54">
@@ -50511,10 +50511,10 @@
         <v>126871</v>
       </c>
       <c r="L54" t="n">
-        <v>58784</v>
+        <v>58819</v>
       </c>
       <c r="M54" t="n">
-        <v>185655</v>
+        <v>185690</v>
       </c>
     </row>
     <row r="55">
@@ -50540,10 +50540,10 @@
         <v>121594</v>
       </c>
       <c r="L55" t="n">
-        <v>15779</v>
+        <v>15788</v>
       </c>
       <c r="M55" t="n">
-        <v>137373</v>
+        <v>137382</v>
       </c>
     </row>
     <row r="56">
@@ -50567,7 +50567,7 @@
       <c r="J56" s="35" t="n"/>
       <c r="K56" s="11" t="n"/>
       <c r="M56" t="n">
-        <v>137787</v>
+        <v>137797</v>
       </c>
     </row>
     <row r="57">

</xml_diff>